<commit_message>
update and jwt token
</commit_message>
<xml_diff>
--- a/Database/Accountdetails.xlsx
+++ b/Database/Accountdetails.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>FirstName</t>
   </si>
@@ -40,10 +40,7 @@
     <t>OpeningDate</t>
   </si>
   <si>
-    <t>Olutunde</t>
-  </si>
-  <si>
-    <t>Sokunbi</t>
+    <t>Tunde</t>
   </si>
   <si>
     <t>Jumoke</t>
@@ -465,13 +462,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3">
         <v>9011762253</v>
       </c>
       <c r="D2" s="3">
-        <v>4567</v>
+        <v>7890</v>
       </c>
       <c r="E2" s="3">
         <v>6000</v>
@@ -482,10 +479,10 @@
     </row>
     <row r="3" ht="17.25" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="3">
         <v>1884197914</v>
@@ -502,10 +499,10 @@
     </row>
     <row r="4" ht="17.25" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C4" s="3">
         <v>3551811021</v>
@@ -522,10 +519,10 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="C5" s="5">
         <v>6415676330</v>

</xml_diff>

<commit_message>
fix token on all transactions
</commit_message>
<xml_diff>
--- a/Database/Accountdetails.xlsx
+++ b/Database/Accountdetails.xlsx
@@ -471,7 +471,7 @@
         <v>7890</v>
       </c>
       <c r="E2" s="3">
-        <v>6000</v>
+        <v>3000</v>
       </c>
       <c r="F2" s="6">
         <v>45432.714594907404</v>
@@ -511,7 +511,7 @@
         <v>2345</v>
       </c>
       <c r="E4" s="3">
-        <v>0</v>
+        <v>24000</v>
       </c>
       <c r="F4" s="6">
         <v>45429.69737268519</v>

</xml_diff>

<commit_message>
add Admin, Auth and User
</commit_message>
<xml_diff>
--- a/Database/Accountdetails.xlsx
+++ b/Database/Accountdetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Documents/Programming Coding/C#/ATMAPI/ATMAPI/ATMAPI/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1DCDA9-E57A-3648-9A8C-FC630B51196D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC12F6D-B20D-0E49-90B6-77BA1B750B83}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>FirstName</t>
   </si>
@@ -40,9 +40,15 @@
     <t>OpeningDate</t>
   </si>
   <si>
+    <t>Role</t>
+  </si>
+  <si>
     <t>Tunde</t>
   </si>
   <si>
+    <t>User</t>
+  </si>
+  <si>
     <t>Jumoke</t>
   </si>
   <si>
@@ -53,6 +59,18 @@
   </si>
   <si>
     <t>Odunlade</t>
+  </si>
+  <si>
+    <t>Adesope</t>
+  </si>
+  <si>
+    <t>Salako</t>
+  </si>
+  <si>
+    <t>5/23/2024 6:35:54 PM</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
@@ -421,10 +439,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -456,13 +474,16 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3">
         <v>9011762253</v>
@@ -471,21 +492,24 @@
         <v>7890</v>
       </c>
       <c r="E2" s="3">
-        <v>3000</v>
+        <v>27000</v>
       </c>
       <c r="F2" s="6">
         <v>45432.714594907404</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3">
-        <v>1884197914</v>
+        <v>1884197911</v>
       </c>
       <c r="D3" s="3">
         <v>2345</v>
@@ -495,14 +519,17 @@
       </c>
       <c r="F3" s="6">
         <v>45432.714594907404</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3">
         <v>3551811021</v>
@@ -511,18 +538,21 @@
         <v>2345</v>
       </c>
       <c r="E4" s="3">
-        <v>24000</v>
+        <v>80000</v>
       </c>
       <c r="F4" s="6">
         <v>45429.69737268519</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5">
         <v>6415676330</v>
@@ -535,6 +565,32 @@
       </c>
       <c r="F5" s="6">
         <v>45432.714594907404</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5">
+        <v>3251134804</v>
+      </c>
+      <c r="D6" s="5">
+        <v>9090</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>